<commit_message>
Made f_name and l_name and + sign
</commit_message>
<xml_diff>
--- a/myproject/telegram_bot/reports/oylik.xlsx
+++ b/myproject/telegram_bot/reports/oylik.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shakh\OneDrive\Документы\GitHub\Uzpar-Oylik\myproject\telegram_bot\reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Phone</t>
   </si>
@@ -34,9 +42,6 @@
     <t>Parol</t>
   </si>
   <si>
-    <t>BahSh</t>
-  </si>
-  <si>
     <t>41wy7d</t>
   </si>
   <si>
@@ -51,27 +56,17 @@
   <si>
     <t>Qwerty</t>
   </si>
+  <si>
+    <t>Bahronov Shaxriyor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -115,52 +110,101 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -362,7 +406,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -381,7 +425,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -411,7 +455,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -437,7 +481,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -463,7 +507,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -489,7 +533,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -515,7 +559,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -541,7 +585,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -567,7 +611,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -593,7 +637,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -619,7 +663,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -632,9 +676,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -651,7 +701,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -670,7 +720,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -696,7 +746,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -722,7 +772,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -748,7 +798,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +824,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -800,7 +850,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -826,7 +876,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -852,7 +902,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -878,7 +928,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -904,7 +954,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -917,9 +967,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -933,7 +989,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -952,7 +1008,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -982,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1008,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1034,7 +1090,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1060,7 +1116,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1086,7 +1142,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1112,7 +1168,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1138,7 +1194,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1220,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1190,7 +1246,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1203,60 +1259,72 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="10" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.67188" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
+    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>998997052366</v>
       </c>
-      <c r="B2" t="s" s="2">
-        <v>7</v>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="3">
         <v>2134322</v>
@@ -1268,19 +1336,18 @@
         <v>2423</v>
       </c>
       <c r="F2" s="3">
-        <f>C2-D2-E2</f>
         <v>2131899</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>8</v>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
+    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>998997055326</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>9</v>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="3">
         <v>324324</v>
@@ -1292,19 +1359,18 @@
         <v>324234</v>
       </c>
       <c r="F3" s="3">
-        <f>C3-D3-E3</f>
         <v>90</v>
       </c>
       <c r="G3" s="3">
         <v>1234</v>
       </c>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
+    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>998914324354</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>10</v>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C4" s="3">
         <v>5334534</v>
@@ -1316,19 +1382,18 @@
         <v>325345</v>
       </c>
       <c r="F4" s="3">
-        <f>C4-D4-E4</f>
         <v>5008847</v>
       </c>
       <c r="G4" s="3">
         <v>4321</v>
       </c>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>998914076350</v>
       </c>
-      <c r="B5" t="s" s="2">
-        <v>11</v>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <v>2000000</v>
@@ -1342,11 +1407,11 @@
       <c r="F5" s="3">
         <v>1300000</v>
       </c>
-      <c r="G5" t="s" s="2">
-        <v>12</v>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
+    <row r="6" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1355,7 +1420,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1364,7 +1429,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
+    <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1373,7 +1438,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1382,7 +1447,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" ht="13.55" customHeight="1">
+    <row r="10" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1393,7 +1458,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>